<commit_message>
week 4 quiz and navigation
</commit_message>
<xml_diff>
--- a/materials/TopicOutline.xlsx
+++ b/materials/TopicOutline.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cimac\OneDrive\Documents\GitHub\statistics\materials\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cimacint\Documents\GitHub\statistics\materials\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="29" documentId="13_ncr:1_{46CFE11A-EC84-4A83-A90F-873A133119B1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{7A03619F-A744-40FF-8462-44BA65F6BFC8}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{295BEC34-9155-4D61-8082-0C3547D9B3A5}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9300" yWindow="60" windowWidth="18840" windowHeight="11724" xr2:uid="{00D72400-CD64-487D-B47C-BF52342530A4}"/>
+    <workbookView xWindow="55725" yWindow="2730" windowWidth="22065" windowHeight="11250" xr2:uid="{00D72400-CD64-487D-B47C-BF52342530A4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -691,17 +691,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87BA1735-2A57-4E12-AB77-93BA6BAC8991}">
   <dimension ref="A1:J85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="H35" sqref="H35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="38.44140625" customWidth="1"/>
-    <col min="4" max="6" width="7.5546875" customWidth="1"/>
+    <col min="3" max="3" width="38.42578125" customWidth="1"/>
+    <col min="4" max="6" width="7.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -733,7 +734,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B2">
         <v>1</v>
       </c>
@@ -747,7 +748,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>1</v>
       </c>
@@ -761,7 +762,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>1</v>
       </c>
@@ -775,7 +776,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>1</v>
       </c>
@@ -789,7 +790,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
         <v>87</v>
       </c>
@@ -797,7 +798,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>2</v>
       </c>
@@ -811,7 +812,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>2</v>
       </c>
@@ -825,7 +826,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>2</v>
       </c>
@@ -836,7 +837,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B10">
         <v>2</v>
       </c>
@@ -847,7 +848,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B11">
         <v>2</v>
       </c>
@@ -861,7 +862,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B12">
         <v>2</v>
       </c>
@@ -875,7 +876,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B13">
         <v>2</v>
       </c>
@@ -889,7 +890,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B14">
         <v>2</v>
       </c>
@@ -906,7 +907,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B15">
         <v>2</v>
       </c>
@@ -920,7 +921,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B16">
         <v>2</v>
       </c>
@@ -931,7 +932,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B17">
         <v>2</v>
       </c>
@@ -942,7 +943,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B18">
         <v>2</v>
       </c>
@@ -953,7 +954,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B19">
         <v>3</v>
       </c>
@@ -964,7 +965,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B20">
         <v>3</v>
       </c>
@@ -978,7 +979,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B21">
         <v>3</v>
       </c>
@@ -989,7 +990,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B22">
         <v>3</v>
       </c>
@@ -1000,7 +1001,7 @@
         <v>2.6</v>
       </c>
     </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B23">
         <v>3</v>
       </c>
@@ -1014,7 +1015,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B24">
         <v>3</v>
       </c>
@@ -1028,7 +1029,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B25">
         <v>3</v>
       </c>
@@ -1042,7 +1043,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B26">
         <v>3</v>
       </c>
@@ -1053,7 +1054,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B27">
         <v>3</v>
       </c>
@@ -1067,7 +1068,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B28">
         <v>3</v>
       </c>
@@ -1078,7 +1079,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B29">
         <v>3</v>
       </c>
@@ -1089,7 +1090,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B30">
         <v>4</v>
       </c>
@@ -1100,7 +1101,7 @@
         <v>3.2</v>
       </c>
     </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B31">
         <v>4</v>
       </c>
@@ -1111,7 +1112,7 @@
         <v>3.3</v>
       </c>
     </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B32">
         <v>4</v>
       </c>
@@ -1122,7 +1123,7 @@
         <v>3.4</v>
       </c>
     </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B33">
         <v>4</v>
       </c>
@@ -1136,7 +1137,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="34" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B34">
         <v>4</v>
       </c>
@@ -1150,7 +1151,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="35" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B35">
         <v>4</v>
       </c>
@@ -1161,7 +1162,7 @@
         <v>3.9</v>
       </c>
     </row>
-    <row r="36" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B36">
         <v>4</v>
       </c>
@@ -1172,7 +1173,7 @@
         <v>6.2</v>
       </c>
     </row>
-    <row r="37" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B37">
         <v>4</v>
       </c>
@@ -1183,7 +1184,7 @@
         <v>6.3</v>
       </c>
     </row>
-    <row r="38" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B38">
         <v>4</v>
       </c>
@@ -1194,7 +1195,7 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="39" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B39">
         <v>4</v>
       </c>
@@ -1205,7 +1206,7 @@
         <v>6.6</v>
       </c>
     </row>
-    <row r="40" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B40">
         <v>4</v>
       </c>
@@ -1216,7 +1217,7 @@
         <v>6.7</v>
       </c>
     </row>
-    <row r="41" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B41">
         <v>4</v>
       </c>
@@ -1227,7 +1228,7 @@
         <v>6.8</v>
       </c>
     </row>
-    <row r="42" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B42">
         <v>4</v>
       </c>
@@ -1238,7 +1239,7 @@
         <v>6.9</v>
       </c>
     </row>
-    <row r="43" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B43">
         <v>4</v>
       </c>
@@ -1249,7 +1250,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="44" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B44">
         <v>4</v>
       </c>
@@ -1260,7 +1261,7 @@
         <v>6.11</v>
       </c>
     </row>
-    <row r="45" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B45">
         <v>4</v>
       </c>
@@ -1271,7 +1272,7 @@
         <v>6.12</v>
       </c>
     </row>
-    <row r="46" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B46">
         <v>4</v>
       </c>
@@ -1282,7 +1283,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="47" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B47">
         <v>4</v>
       </c>
@@ -1293,7 +1294,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="48" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B48">
         <v>4</v>
       </c>
@@ -1304,7 +1305,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="49" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B49">
         <v>4</v>
       </c>
@@ -1315,7 +1316,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="50" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B50">
         <v>5</v>
       </c>
@@ -1326,7 +1327,7 @@
         <v>10.4</v>
       </c>
     </row>
-    <row r="51" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B51">
         <v>5</v>
       </c>
@@ -1337,7 +1338,7 @@
         <v>10.5</v>
       </c>
     </row>
-    <row r="52" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B52">
         <v>5</v>
       </c>
@@ -1348,7 +1349,7 @@
         <v>10.6</v>
       </c>
     </row>
-    <row r="53" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B53">
         <v>5</v>
       </c>
@@ -1359,27 +1360,27 @@
         <v>69</v>
       </c>
     </row>
-    <row r="54" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C54" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="55" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C55" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="56" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C56" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="57" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C57" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="61" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="61" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B61">
         <v>6</v>
       </c>
@@ -1390,7 +1391,7 @@
         <v>7.2</v>
       </c>
     </row>
-    <row r="62" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="62" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B62">
         <v>6</v>
       </c>
@@ -1401,7 +1402,7 @@
         <v>7.4</v>
       </c>
     </row>
-    <row r="63" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="63" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B63">
         <v>6</v>
       </c>
@@ -1412,7 +1413,7 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="64" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="64" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B64">
         <v>6</v>
       </c>
@@ -1423,7 +1424,7 @@
         <v>7.6</v>
       </c>
     </row>
-    <row r="65" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="65" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B65">
         <v>6</v>
       </c>
@@ -1434,7 +1435,7 @@
         <v>7.7</v>
       </c>
     </row>
-    <row r="70" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="70" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C70" t="s">
         <v>75</v>
       </c>
@@ -1442,7 +1443,7 @@
         <v>12.2</v>
       </c>
     </row>
-    <row r="71" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="71" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C71" t="s">
         <v>67</v>
       </c>
@@ -1450,7 +1451,7 @@
         <v>12.3</v>
       </c>
     </row>
-    <row r="72" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="72" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C72" t="s">
         <v>76</v>
       </c>
@@ -1458,7 +1459,7 @@
         <v>12.4</v>
       </c>
     </row>
-    <row r="73" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="73" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C73" t="s">
         <v>77</v>
       </c>
@@ -1466,7 +1467,7 @@
         <v>12.5</v>
       </c>
     </row>
-    <row r="74" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="74" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C74" t="s">
         <v>78</v>
       </c>
@@ -1474,27 +1475,27 @@
         <v>12.7</v>
       </c>
     </row>
-    <row r="75" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="75" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C75" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="76" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="76" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C76" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="77" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="77" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C77" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="78" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="78" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C78" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="82" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="82" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C82" t="s">
         <v>82</v>
       </c>
@@ -1502,7 +1503,7 @@
         <v>13.2</v>
       </c>
     </row>
-    <row r="83" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="83" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C83" t="s">
         <v>67</v>
       </c>
@@ -1510,12 +1511,12 @@
         <v>13.4</v>
       </c>
     </row>
-    <row r="84" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="84" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C84" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="85" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="85" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C85" t="s">
         <v>84</v>
       </c>

</xml_diff>